<commit_message>
Some API changes and UI pushed
</commit_message>
<xml_diff>
--- a/EPLPredictorBackend/PLFixtures.xlsx
+++ b/EPLPredictorBackend/PLFixtures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="56">
   <si>
     <t>Home Team</t>
   </si>
@@ -46,55 +46,52 @@
     <t>Dec 04 2020</t>
   </si>
   <si>
+    <t>Leicester</t>
+  </si>
+  <si>
+    <t>Dec 26 2020</t>
+  </si>
+  <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Sheffield United</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Leeds</t>
+  </si>
+  <si>
+    <t>Dec 27 2020</t>
+  </si>
+  <si>
+    <t>West Ham</t>
+  </si>
+  <si>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
     <t>Wolverhampton Wanderers</t>
-  </si>
-  <si>
-    <t>Dec 21 2020</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>West Ham</t>
-  </si>
-  <si>
-    <t>Leicester</t>
-  </si>
-  <si>
-    <t>Dec 26 2020</t>
-  </si>
-  <si>
-    <t>Crystal Palace</t>
-  </si>
-  <si>
-    <t>Fulham</t>
-  </si>
-  <si>
-    <t>Southampton</t>
-  </si>
-  <si>
-    <t>Arsenal</t>
-  </si>
-  <si>
-    <t>Sheffield United</t>
-  </si>
-  <si>
-    <t>Everton</t>
-  </si>
-  <si>
-    <t>Leeds</t>
-  </si>
-  <si>
-    <t>Dec 27 2020</t>
-  </si>
-  <si>
-    <t>Brighton</t>
-  </si>
-  <si>
-    <t>Liverpool</t>
-  </si>
-  <si>
-    <t>West Bromwich Albion</t>
   </si>
   <si>
     <t>Tottenham</t>
@@ -516,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C246"/>
+  <dimension ref="A1:C244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,10 +565,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -579,10 +576,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -590,131 +587,131 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
         <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -722,10 +719,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -733,35 +730,35 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -769,7 +766,7 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -777,10 +774,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
@@ -788,10 +785,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
         <v>30</v>
@@ -799,10 +796,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
@@ -810,98 +807,98 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
         <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
@@ -909,10 +906,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
         <v>31</v>
@@ -920,76 +917,76 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
         <v>32</v>
@@ -997,10 +994,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
         <v>32</v>
@@ -1008,10 +1005,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
@@ -1019,10 +1016,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
         <v>33</v>
@@ -1030,98 +1027,98 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
         <v>13</v>
-      </c>
-      <c r="B55" t="s">
-        <v>3</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
@@ -1129,10 +1126,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>34</v>
@@ -1140,43 +1137,43 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C60" t="s">
         <v>35</v>
@@ -1184,10 +1181,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
         <v>35</v>
@@ -1195,43 +1192,43 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
         <v>36</v>
@@ -1239,10 +1236,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C66" t="s">
         <v>36</v>
@@ -1250,98 +1247,98 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
         <v>17</v>
       </c>
       <c r="C72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C75" t="s">
         <v>37</v>
@@ -1349,10 +1346,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
         <v>37</v>
@@ -1360,24 +1357,24 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1385,40 +1382,40 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C79" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C80" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
         <v>38</v>
@@ -1426,10 +1423,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C83" t="s">
         <v>38</v>
@@ -1437,21 +1434,21 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B84" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
@@ -1459,10 +1456,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C86" t="s">
         <v>39</v>
@@ -1470,98 +1467,98 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C90" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C92" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C95" t="s">
         <v>40</v>
@@ -1569,10 +1566,10 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C96" t="s">
         <v>40</v>
@@ -1580,57 +1577,57 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C98" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C99" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B101" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C101" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1641,37 +1638,37 @@
         <v>25</v>
       </c>
       <c r="C102" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C104" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C105" t="s">
         <v>41</v>
@@ -1679,10 +1676,10 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B106" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C106" t="s">
         <v>41</v>
@@ -1690,98 +1687,98 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B109" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B110" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C110" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B112" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C112" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C113" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B114" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C114" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B115" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C115" t="s">
         <v>42</v>
@@ -1789,10 +1786,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B116" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C116" t="s">
         <v>42</v>
@@ -1803,95 +1800,95 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C117" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C118" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C119" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C120" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B122" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C124" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B125" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C125" t="s">
         <v>43</v>
@@ -1899,10 +1896,10 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C126" t="s">
         <v>43</v>
@@ -1910,98 +1907,98 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B127" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C127" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B128" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C128" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B129" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C129" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B130" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C130" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B131" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C131" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C132" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B133" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B134" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C134" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>15</v>
+      </c>
+      <c r="B135" t="s">
         <v>26</v>
-      </c>
-      <c r="B135" t="s">
-        <v>8</v>
       </c>
       <c r="C135" t="s">
         <v>44</v>
@@ -2009,10 +2006,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B136" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C136" t="s">
         <v>44</v>
@@ -2020,98 +2017,98 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B137" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C137" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B138" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C139" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140" t="s">
         <v>17</v>
       </c>
-      <c r="B140" t="s">
-        <v>6</v>
-      </c>
       <c r="C140" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C141" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C142" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B143" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C143" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B144" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C144" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C145" t="s">
         <v>45</v>
@@ -2119,10 +2116,10 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s">
         <v>10</v>
-      </c>
-      <c r="B146" t="s">
-        <v>25</v>
       </c>
       <c r="C146" t="s">
         <v>45</v>
@@ -2130,98 +2127,98 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B147" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B148" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C148" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
+        <v>23</v>
+      </c>
+      <c r="B149" t="s">
         <v>16</v>
       </c>
-      <c r="B149" t="s">
-        <v>4</v>
-      </c>
       <c r="C149" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B150" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C150" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C151" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B152" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C152" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B153" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C153" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B154" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C154" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B155" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C155" t="s">
         <v>46</v>
@@ -2229,10 +2226,10 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
+        <v>7</v>
+      </c>
+      <c r="B156" t="s">
         <v>13</v>
-      </c>
-      <c r="B156" t="s">
-        <v>19</v>
       </c>
       <c r="C156" t="s">
         <v>46</v>
@@ -2240,98 +2237,98 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B157" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C157" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B158" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C158" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B159" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C159" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B160" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
+        <v>4</v>
+      </c>
+      <c r="B161" t="s">
         <v>22</v>
       </c>
-      <c r="B161" t="s">
-        <v>20</v>
-      </c>
       <c r="C161" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B162" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C162" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B163" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C163" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B164" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C164" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
+        <v>22</v>
+      </c>
+      <c r="B165" t="s">
         <v>18</v>
-      </c>
-      <c r="B165" t="s">
-        <v>3</v>
       </c>
       <c r="C165" t="s">
         <v>47</v>
@@ -2339,10 +2336,10 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B166" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C166" t="s">
         <v>47</v>
@@ -2350,98 +2347,98 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B167" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C167" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B168" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C168" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B169" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B170" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C170" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B171" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C171" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B172" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B173" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C173" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C174" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B175" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C175" t="s">
         <v>48</v>
@@ -2449,10 +2446,10 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B176" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C176" t="s">
         <v>48</v>
@@ -2460,98 +2457,98 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B177" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C177" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B178" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C178" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B179" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C179" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C180" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C181" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B182" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C182" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B183" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C183" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B184" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C184" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
+        <v>15</v>
+      </c>
+      <c r="B185" t="s">
         <v>18</v>
-      </c>
-      <c r="B185" t="s">
-        <v>16</v>
       </c>
       <c r="C185" t="s">
         <v>49</v>
@@ -2559,10 +2556,10 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B186" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C186" t="s">
         <v>49</v>
@@ -2570,98 +2567,98 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B187" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C187" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B188" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C188" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B189" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C189" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B190" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C190" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
+        <v>6</v>
+      </c>
+      <c r="B191" t="s">
         <v>14</v>
       </c>
-      <c r="B191" t="s">
-        <v>16</v>
-      </c>
       <c r="C191" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C192" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B193" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C193" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B194" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C194" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B195" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C195" t="s">
         <v>50</v>
@@ -2669,10 +2666,10 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B196" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C196" t="s">
         <v>50</v>
@@ -2680,98 +2677,98 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B197" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C197" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B198" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C198" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B199" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C199" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C200" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B201" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C201" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B202" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C202" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B203" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C203" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B204" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C204" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B205" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C205" t="s">
         <v>51</v>
@@ -2779,10 +2776,10 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B206" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C206" t="s">
         <v>51</v>
@@ -2790,95 +2787,95 @@
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B207" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C207" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B208" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C208" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B209" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C209" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B210" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C210" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B211" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C211" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B212" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C212" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B213" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C213" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B214" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C214" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B215" t="s">
         <v>21</v>
@@ -2889,10 +2886,10 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B216" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C216" t="s">
         <v>52</v>
@@ -2900,43 +2897,43 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B217" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C217" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B218" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C218" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B219" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C219" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B220" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C220" t="s">
         <v>53</v>
@@ -2944,10 +2941,10 @@
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B221" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C221" t="s">
         <v>53</v>
@@ -2955,43 +2952,43 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B222" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C222" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B223" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C223" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B224" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C224" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B225" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C225" t="s">
         <v>54</v>
@@ -2999,10 +2996,10 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B226" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C226" t="s">
         <v>54</v>
@@ -3010,98 +3007,98 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B227" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C227" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B228" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C228" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B229" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C229" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B230" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C230" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B231" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C231" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B232" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C232" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B233" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C233" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B234" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C234" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B235" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C235" t="s">
         <v>55</v>
@@ -3109,10 +3106,10 @@
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B236" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C236" t="s">
         <v>55</v>
@@ -3120,112 +3117,90 @@
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B237" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B238" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C238" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B239" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C239" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B240" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C240" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B241" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C241" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B242" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C242" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B243" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C243" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B244" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C244" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
-      <c r="A245" t="s">
-        <v>13</v>
-      </c>
-      <c r="B245" t="s">
-        <v>18</v>
-      </c>
-      <c r="C245" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
-      <c r="A246" t="s">
-        <v>10</v>
-      </c>
-      <c r="B246" t="s">
-        <v>4</v>
-      </c>
-      <c r="C246" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed weight and added screenshots for this gameweek
</commit_message>
<xml_diff>
--- a/EPLPredictorBackend/PLFixtures.xlsx
+++ b/EPLPredictorBackend/PLFixtures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="54">
   <si>
     <t>Home Team</t>
   </si>
@@ -46,64 +46,58 @@
     <t>Dec 04 2020</t>
   </si>
   <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
     <t>Leicester</t>
   </si>
   <si>
-    <t>Dec 26 2020</t>
-  </si>
-  <si>
-    <t>Crystal Palace</t>
+    <t>Dec 28 2020</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Dec 29 2020</t>
+  </si>
+  <si>
+    <t>Sheffield United</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>West Ham</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>Leeds</t>
+  </si>
+  <si>
+    <t>Wolverhampton Wanderers</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
   </si>
   <si>
     <t>Fulham</t>
   </si>
   <si>
-    <t>Southampton</t>
-  </si>
-  <si>
-    <t>Arsenal</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Sheffield United</t>
-  </si>
-  <si>
-    <t>Everton</t>
-  </si>
-  <si>
-    <t>Leeds</t>
-  </si>
-  <si>
-    <t>Dec 27 2020</t>
-  </si>
-  <si>
-    <t>West Ham</t>
-  </si>
-  <si>
-    <t>Brighton</t>
+    <t>Dec 30 2020</t>
   </si>
   <si>
     <t>Liverpool</t>
-  </si>
-  <si>
-    <t>West Bromwich Albion</t>
-  </si>
-  <si>
-    <t>Wolverhampton Wanderers</t>
-  </si>
-  <si>
-    <t>Tottenham</t>
-  </si>
-  <si>
-    <t>Dec 28 2020</t>
-  </si>
-  <si>
-    <t>Dec 29 2020</t>
-  </si>
-  <si>
-    <t>Dec 30 2020</t>
   </si>
   <si>
     <t>Jan 02 2021</t>
@@ -513,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C244"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,32 +562,32 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -604,114 +598,114 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
@@ -719,10 +713,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -730,10 +724,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -741,10 +735,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -752,7 +746,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
@@ -763,120 +757,120 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -884,10 +878,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
         <v>30</v>
@@ -895,10 +889,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
@@ -909,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
         <v>31</v>
@@ -917,10 +911,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
         <v>13</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
@@ -928,10 +922,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
         <v>31</v>
@@ -939,10 +933,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
         <v>31</v>
@@ -950,10 +944,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
         <v>31</v>
@@ -961,10 +955,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
         <v>31</v>
@@ -972,10 +966,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
         <v>31</v>
@@ -983,24 +977,24 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1008,62 +1002,62 @@
         <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="B46" t="s">
-        <v>18</v>
-      </c>
       <c r="C46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s">
         <v>23</v>
-      </c>
-      <c r="B50" t="s">
-        <v>4</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
@@ -1071,10 +1065,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
@@ -1082,10 +1076,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
         <v>33</v>
@@ -1093,10 +1087,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
@@ -1104,10 +1098,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C54" t="s">
         <v>33</v>
@@ -1115,10 +1109,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
         <v>34</v>
@@ -1126,10 +1120,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C56" t="s">
         <v>34</v>
@@ -1137,10 +1131,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
         <v>34</v>
@@ -1148,10 +1142,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C58" t="s">
         <v>34</v>
@@ -1159,10 +1153,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
         <v>34</v>
@@ -1170,142 +1164,142 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B60" t="s">
         <v>25</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
         <v>21</v>
       </c>
-      <c r="B69" t="s">
-        <v>23</v>
-      </c>
       <c r="C69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C72" t="s">
         <v>36</v>
@@ -1313,10 +1307,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
         <v>36</v>
@@ -1324,10 +1318,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
         <v>36</v>
@@ -1338,7 +1332,7 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
         <v>37</v>
@@ -1349,7 +1343,7 @@
         <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C76" t="s">
         <v>37</v>
@@ -1357,10 +1351,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C77" t="s">
         <v>37</v>
@@ -1368,10 +1362,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
         <v>37</v>
@@ -1379,10 +1373,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
         <v>37</v>
@@ -1390,10 +1384,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
         <v>37</v>
@@ -1401,10 +1395,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C81" t="s">
         <v>37</v>
@@ -1412,24 +1406,24 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B82" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C82" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1437,32 +1431,32 @@
         <v>23</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1470,384 +1464,384 @@
         <v>13</v>
       </c>
       <c r="B87" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C89" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C90" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C94" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C96" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
+        <v>25</v>
+      </c>
+      <c r="B99" t="s">
         <v>18</v>
       </c>
-      <c r="B99" t="s">
-        <v>13</v>
-      </c>
       <c r="C99" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
         <v>24</v>
       </c>
-      <c r="B103" t="s">
-        <v>4</v>
-      </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C104" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B106" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C107" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C110" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C112" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B113" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B114" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C114" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C116" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C117" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B119" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C119" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
+        <v>18</v>
+      </c>
+      <c r="B121" t="s">
         <v>19</v>
       </c>
-      <c r="B121" t="s">
-        <v>7</v>
-      </c>
       <c r="C121" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1855,142 +1849,142 @@
         <v>24</v>
       </c>
       <c r="B122" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C122" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C123" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B124" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C124" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C126" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
+        <v>14</v>
+      </c>
+      <c r="B127" t="s">
         <v>3</v>
       </c>
-      <c r="B127" t="s">
-        <v>15</v>
-      </c>
       <c r="C127" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B128" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B129" t="s">
         <v>13</v>
       </c>
       <c r="C129" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C130" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C131" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B132" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C132" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B133" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C133" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B134" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C134" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1998,219 +1992,219 @@
         <v>15</v>
       </c>
       <c r="B135" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B136" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C136" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B137" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C138" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C139" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B140" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C140" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B141" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C141" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B142" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C142" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
+        <v>21</v>
+      </c>
+      <c r="B143" t="s">
         <v>14</v>
       </c>
-      <c r="B143" t="s">
-        <v>22</v>
-      </c>
       <c r="C143" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B144" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C144" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B145" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C145" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C146" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C147" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B148" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C148" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B149" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
+        <v>11</v>
+      </c>
+      <c r="B150" t="s">
         <v>6</v>
       </c>
-      <c r="B150" t="s">
-        <v>25</v>
-      </c>
       <c r="C150" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B151" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B152" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C152" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B153" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C153" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B154" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C154" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2218,230 +2212,230 @@
         <v>15</v>
       </c>
       <c r="B155" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C155" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C156" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B157" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C157" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B158" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C158" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B159" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B160" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C160" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B161" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C161" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B162" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B163" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C163" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C164" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B165" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C165" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B166" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C166" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B167" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C167" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B168" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C168" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B169" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C169" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B170" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C170" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B171" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C171" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C172" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B173" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C173" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B174" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C174" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C175" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -2449,98 +2443,98 @@
         <v>7</v>
       </c>
       <c r="B176" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C176" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B177" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C177" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B178" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C178" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B179" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C179" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B180" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C180" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B181" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C181" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B182" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C182" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C183" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B184" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C184" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2548,21 +2542,21 @@
         <v>15</v>
       </c>
       <c r="B185" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C185" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B186" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C186" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2570,197 +2564,197 @@
         <v>13</v>
       </c>
       <c r="B187" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C187" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C188" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B189" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C190" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B191" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C191" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B192" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C192" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B193" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C193" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B194" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C194" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B195" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C195" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B196" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C196" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B197" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C197" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B198" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C198" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B199" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C199" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B200" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C200" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B201" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C201" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B202" t="s">
         <v>10</v>
       </c>
       <c r="C202" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B203" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C203" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B204" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C204" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -2768,62 +2762,62 @@
         <v>15</v>
       </c>
       <c r="B205" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C205" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B206" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C206" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B207" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C207" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B208" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C208" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B209" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C209" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B210" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C210" t="s">
         <v>51</v>
@@ -2831,10 +2825,10 @@
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211" t="s">
         <v>6</v>
-      </c>
-      <c r="B211" t="s">
-        <v>16</v>
       </c>
       <c r="C211" t="s">
         <v>51</v>
@@ -2842,10 +2836,10 @@
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B212" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C212" t="s">
         <v>51</v>
@@ -2853,10 +2847,10 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B213" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C213" t="s">
         <v>51</v>
@@ -2864,10 +2858,10 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B214" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C214" t="s">
         <v>51</v>
@@ -2875,10 +2869,10 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B215" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C215" t="s">
         <v>52</v>
@@ -2889,7 +2883,7 @@
         <v>3</v>
       </c>
       <c r="B216" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C216" t="s">
         <v>52</v>
@@ -2897,10 +2891,10 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B217" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C217" t="s">
         <v>52</v>
@@ -2908,10 +2902,10 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B218" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C218" t="s">
         <v>52</v>
@@ -2919,7 +2913,7 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B219" t="s">
         <v>23</v>
@@ -2930,13 +2924,13 @@
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B220" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C220" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -2944,263 +2938,153 @@
         <v>8</v>
       </c>
       <c r="B221" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C221" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B222" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C222" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B223" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C223" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B224" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C224" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B225" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C225" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B226" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C226" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B227" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B228" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C228" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B229" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C229" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B230" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C230" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B231" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C231" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B232" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C232" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B233" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C233" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B234" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C234" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" t="s">
-        <v>15</v>
-      </c>
-      <c r="B235" t="s">
-        <v>22</v>
-      </c>
-      <c r="C235" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236" t="s">
-        <v>7</v>
-      </c>
-      <c r="B236" t="s">
-        <v>16</v>
-      </c>
-      <c r="C236" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
-      <c r="A237" t="s">
-        <v>13</v>
-      </c>
-      <c r="B237" t="s">
-        <v>8</v>
-      </c>
-      <c r="C237" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" t="s">
-        <v>19</v>
-      </c>
-      <c r="B238" t="s">
-        <v>24</v>
-      </c>
-      <c r="C238" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" t="s">
-        <v>10</v>
-      </c>
-      <c r="B239" t="s">
-        <v>26</v>
-      </c>
-      <c r="C239" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" t="s">
-        <v>23</v>
-      </c>
-      <c r="B240" t="s">
-        <v>12</v>
-      </c>
-      <c r="C240" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
-      <c r="A241" t="s">
-        <v>6</v>
-      </c>
-      <c r="B241" t="s">
-        <v>18</v>
-      </c>
-      <c r="C241" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
-      <c r="A242" t="s">
-        <v>17</v>
-      </c>
-      <c r="B242" t="s">
-        <v>3</v>
-      </c>
-      <c r="C242" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243" t="s">
-        <v>21</v>
-      </c>
-      <c r="B243" t="s">
-        <v>14</v>
-      </c>
-      <c r="C243" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244" t="s">
-        <v>25</v>
-      </c>
-      <c r="B244" t="s">
-        <v>4</v>
-      </c>
-      <c r="C244" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Screenshots for gameweek 18
</commit_message>
<xml_diff>
--- a/EPLPredictorBackend/PLFixtures.xlsx
+++ b/EPLPredictorBackend/PLFixtures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="61">
   <si>
     <t>Home Team</t>
   </si>
@@ -25,88 +25,106 @@
     <t>Date</t>
   </si>
   <si>
+    <t>Aston Villa</t>
+  </si>
+  <si>
+    <t>Newcastle United</t>
+  </si>
+  <si>
+    <t>Dec 04 2020</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
+    <t>Dec 28 2020</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Dec 30 2020</t>
+  </si>
+  <si>
     <t>Burnley</t>
   </si>
   <si>
+    <t>Jan 03 2021</t>
+  </si>
+  <si>
+    <t>Sheffield United</t>
+  </si>
+  <si>
+    <t>Jan 12 2021</t>
+  </si>
+  <si>
+    <t>Wolverhampton Wanderers</t>
+  </si>
+  <si>
     <t>Manchester United</t>
   </si>
   <si>
-    <t>Sep 12 2020</t>
-  </si>
-  <si>
-    <t>Manchester City</t>
-  </si>
-  <si>
-    <t>Aston Villa</t>
-  </si>
-  <si>
-    <t>Newcastle United</t>
-  </si>
-  <si>
-    <t>Dec 04 2020</t>
-  </si>
-  <si>
-    <t>Everton</t>
-  </si>
-  <si>
-    <t>Dec 28 2020</t>
-  </si>
-  <si>
-    <t>Tottenham</t>
-  </si>
-  <si>
-    <t>Fulham</t>
-  </si>
-  <si>
-    <t>Dec 30 2020</t>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Jan 13 2021</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Jan 14 2021</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Jan 15 2021</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>Jan 16 2021</t>
+  </si>
+  <si>
+    <t>Leeds</t>
   </si>
   <si>
     <t>West Ham</t>
   </si>
   <si>
-    <t>Jan 02 2021</t>
-  </si>
-  <si>
     <t>Leicester</t>
   </si>
   <si>
     <t>Southampton</t>
   </si>
   <si>
+    <t>Jan 17 2021</t>
+  </si>
+  <si>
     <t>Liverpool</t>
   </si>
   <si>
-    <t>Leeds</t>
-  </si>
-  <si>
-    <t>West Bromwich Albion</t>
-  </si>
-  <si>
-    <t>Arsenal</t>
-  </si>
-  <si>
-    <t>Brighton</t>
-  </si>
-  <si>
-    <t>Wolverhampton Wanderers</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Crystal Palace</t>
-  </si>
-  <si>
-    <t>Sheffield United</t>
-  </si>
-  <si>
-    <t>Jan 12 2021</t>
-  </si>
-  <si>
-    <t>Jan 13 2021</t>
-  </si>
-  <si>
-    <t>Jan 16 2021</t>
+    <t>Jan 18 2021</t>
+  </si>
+  <si>
+    <t>Jan 19 2021</t>
+  </si>
+  <si>
+    <t>Jan 20 2021</t>
+  </si>
+  <si>
+    <t>Jan 21 2021</t>
   </si>
   <si>
     <t>Jan 26 2021</t>
@@ -115,7 +133,13 @@
     <t>Jan 27 2021</t>
   </si>
   <si>
+    <t>Jan 28 2021</t>
+  </si>
+  <si>
     <t>Jan 30 2021</t>
+  </si>
+  <si>
+    <t>Jan 31 2021</t>
   </si>
   <si>
     <t>Feb 02 2021</t>
@@ -504,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -540,601 +564,601 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
         <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1142,32 +1166,32 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1178,1085 +1202,1085 @@
         <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
         <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C75" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B76" t="s">
         <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C80" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" t="s">
         <v>6</v>
       </c>
-      <c r="B83" t="s">
-        <v>12</v>
-      </c>
       <c r="C83" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C85" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B88" t="s">
         <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C89" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C90" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C92" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C93" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C97" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C98" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C99" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101" t="s">
         <v>6</v>
       </c>
-      <c r="B101" t="s">
-        <v>15</v>
-      </c>
       <c r="C101" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B102" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C102" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B103" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C103" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B104" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C104" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C105" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B106" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B109" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C112" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C113" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C114" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C115" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B116" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C116" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B117" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C117" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B118" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C119" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B120" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C120" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C121" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C122" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B123" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C123" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B124" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C125" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B126" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C127" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C128" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C130" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C131" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B132" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C132" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B134" t="s">
         <v>18</v>
       </c>
       <c r="C134" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C135" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C136" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B137" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C137" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B139" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B140" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C140" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B141" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C141" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C143" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B144" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C144" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C145" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B146" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C146" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C147" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C148" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C149" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B150" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C150" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B151" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C151" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B152" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C152" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B153" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C153" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
+        <v>17</v>
+      </c>
+      <c r="B154" t="s">
         <v>12</v>
       </c>
-      <c r="B154" t="s">
-        <v>4</v>
-      </c>
       <c r="C154" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C155" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B156" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C156" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C157" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B158" t="s">
         <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
         <v>25</v>
       </c>
-      <c r="B159" t="s">
-        <v>23</v>
-      </c>
       <c r="C159" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -2264,340 +2288,340 @@
         <v>10</v>
       </c>
       <c r="B160" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C160" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B161" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C161" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B162" t="s">
         <v>21</v>
       </c>
       <c r="C162" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
+        <v>32</v>
+      </c>
+      <c r="B163" t="s">
         <v>4</v>
       </c>
-      <c r="B163" t="s">
-        <v>3</v>
-      </c>
       <c r="C163" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B164" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C164" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" t="s">
         <v>18</v>
       </c>
-      <c r="B165" t="s">
-        <v>26</v>
-      </c>
       <c r="C165" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B166" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C166" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B167" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C167" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B168" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C168" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B169" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C169" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B170" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C170" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B171" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C171" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B172" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C172" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B173" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C173" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C174" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B175" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C175" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B176" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C176" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B177" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C177" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B178" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C178" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B179" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C179" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C180" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B181" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C181" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
+        <v>29</v>
+      </c>
+      <c r="B182" t="s">
         <v>4</v>
       </c>
-      <c r="B182" t="s">
-        <v>19</v>
-      </c>
       <c r="C182" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B183" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C183" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B184" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C184" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B185" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C185" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B186" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C186" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B187" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C187" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C188" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B189" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C189" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B190" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C190" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2605,109 +2629,109 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C191" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B192" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C192" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B193" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C193" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C194" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B195" t="s">
         <v>10</v>
       </c>
       <c r="C195" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B196" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C196" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C197" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B198" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C198" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B199" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C199" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B200" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C200" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -2715,285 +2739,186 @@
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C201" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B202" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C202" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B203" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C203" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C204" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B205" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C205" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B206" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C206" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B207" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C207" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B208" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C208" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B209" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C209" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B210" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B211" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C211" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B212" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C212" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B213" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C213" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B214" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C214" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
+        <v>14</v>
+      </c>
+      <c r="B215" t="s">
         <v>12</v>
       </c>
-      <c r="B215" t="s">
-        <v>7</v>
-      </c>
       <c r="C215" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B216" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C216" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B217" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C217" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" t="s">
-        <v>7</v>
-      </c>
-      <c r="B218" t="s">
-        <v>25</v>
-      </c>
-      <c r="C218" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" t="s">
-        <v>13</v>
-      </c>
-      <c r="B219" t="s">
-        <v>8</v>
-      </c>
-      <c r="C219" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" t="s">
-        <v>20</v>
-      </c>
-      <c r="B220" t="s">
-        <v>21</v>
-      </c>
-      <c r="C220" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" t="s">
-        <v>17</v>
-      </c>
-      <c r="B221" t="s">
-        <v>12</v>
-      </c>
-      <c r="C221" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
-      <c r="A222" t="s">
-        <v>19</v>
-      </c>
-      <c r="B222" t="s">
-        <v>26</v>
-      </c>
-      <c r="C222" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" t="s">
-        <v>6</v>
-      </c>
-      <c r="B223" t="s">
-        <v>10</v>
-      </c>
-      <c r="C223" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" t="s">
-        <v>27</v>
-      </c>
-      <c r="B224" t="s">
-        <v>3</v>
-      </c>
-      <c r="C224" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3">
-      <c r="A225" t="s">
-        <v>15</v>
-      </c>
-      <c r="B225" t="s">
-        <v>18</v>
-      </c>
-      <c r="C225" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
-      <c r="A226" t="s">
-        <v>24</v>
-      </c>
-      <c r="B226" t="s">
-        <v>4</v>
-      </c>
-      <c r="C226" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Screenshots for GW21 and 22
</commit_message>
<xml_diff>
--- a/EPLPredictorBackend/PLFixtures.xlsx
+++ b/EPLPredictorBackend/PLFixtures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="57">
   <si>
     <t>Home Team</t>
   </si>
@@ -64,100 +64,115 @@
     <t>Jan 20 2021</t>
   </si>
   <si>
+    <t>Sheffield United</t>
+  </si>
+  <si>
+    <t>West Bromwich Albion</t>
+  </si>
+  <si>
+    <t>Feb 02 2021</t>
+  </si>
+  <si>
+    <t>Wolverhampton Wanderers</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Manchester United</t>
+  </si>
+  <si>
     <t>Newcastle United</t>
   </si>
   <si>
-    <t>Jan 26 2021</t>
-  </si>
-  <si>
     <t>Crystal Palace</t>
   </si>
   <si>
+    <t>Feb 03 2021</t>
+  </si>
+  <si>
+    <t>Leicester</t>
+  </si>
+  <si>
     <t>West Ham</t>
   </si>
   <si>
-    <t>West Bromwich Albion</t>
-  </si>
-  <si>
-    <t>Arsenal</t>
-  </si>
-  <si>
-    <t>Jan 27 2021</t>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Brighton</t>
   </si>
   <si>
     <t>Chelsea</t>
   </si>
   <si>
-    <t>Wolverhampton Wanderers</t>
-  </si>
-  <si>
-    <t>Brighton</t>
-  </si>
-  <si>
-    <t>Leicester</t>
-  </si>
-  <si>
-    <t>Manchester United</t>
-  </si>
-  <si>
-    <t>Sheffield United</t>
-  </si>
-  <si>
-    <t>Liverpool</t>
-  </si>
-  <si>
-    <t>Jan 28 2021</t>
-  </si>
-  <si>
-    <t>Jan 30 2021</t>
-  </si>
-  <si>
-    <t>Jan 31 2021</t>
-  </si>
-  <si>
-    <t>Feb 02 2021</t>
-  </si>
-  <si>
-    <t>Feb 03 2021</t>
+    <t>Feb 04 2021</t>
   </si>
   <si>
     <t>Feb 06 2021</t>
   </si>
   <si>
+    <t>Feb 07 2021</t>
+  </si>
+  <si>
+    <t>Feb 08 2021</t>
+  </si>
+  <si>
     <t>Feb 13 2021</t>
   </si>
   <si>
+    <t>Feb 14 2021</t>
+  </si>
+  <si>
+    <t>Feb 15 2021</t>
+  </si>
+  <si>
+    <t>Feb 19 2021</t>
+  </si>
+  <si>
     <t>Feb 20 2021</t>
   </si>
   <si>
+    <t>Feb 21 2021</t>
+  </si>
+  <si>
+    <t>Feb 22 2021</t>
+  </si>
+  <si>
+    <t>Feb 26 2021</t>
+  </si>
+  <si>
     <t>Feb 27 2021</t>
   </si>
   <si>
-    <t>Mar 06 2021</t>
-  </si>
-  <si>
-    <t>Mar 13 2021</t>
-  </si>
-  <si>
-    <t>Mar 20 2021</t>
-  </si>
-  <si>
-    <t>Apr 03 2021</t>
-  </si>
-  <si>
-    <t>Apr 10 2021</t>
-  </si>
-  <si>
-    <t>Apr 17 2021</t>
-  </si>
-  <si>
-    <t>Apr 24 2021</t>
-  </si>
-  <si>
-    <t>May 01 2021</t>
-  </si>
-  <si>
-    <t>May 08 2021</t>
+    <t>Feb 28 2021</t>
+  </si>
+  <si>
+    <t>Mar 05 2021</t>
+  </si>
+  <si>
+    <t>Mar 12 2021</t>
+  </si>
+  <si>
+    <t>Mar 19 2021</t>
+  </si>
+  <si>
+    <t>Apr 02 2021</t>
+  </si>
+  <si>
+    <t>Apr 09 2021</t>
+  </si>
+  <si>
+    <t>Apr 16 2021</t>
+  </si>
+  <si>
+    <t>Apr 23 2021</t>
+  </si>
+  <si>
+    <t>Apr 30 2021</t>
+  </si>
+  <si>
+    <t>May 07 2021</t>
   </si>
   <si>
     <t>May 11 2021</t>
@@ -166,10 +181,10 @@
     <t>May 12 2021</t>
   </si>
   <si>
-    <t>May 15 2021</t>
-  </si>
-  <si>
-    <t>May 23 2021</t>
+    <t>May 14 2021</t>
+  </si>
+  <si>
+    <t>May 22 2021</t>
   </si>
 </sst>
 </file>
@@ -501,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -578,43 +593,43 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -622,43 +637,43 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -669,7 +684,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -685,10 +700,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
@@ -696,10 +711,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>31</v>
@@ -707,10 +722,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
         <v>31</v>
@@ -718,10 +733,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -729,10 +744,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -740,32 +755,32 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -773,10 +788,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -784,112 +799,112 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
         <v>6</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -897,505 +912,505 @@
         <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
         <v>7</v>
       </c>
-      <c r="B61" t="s">
-        <v>28</v>
-      </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
         <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C71" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C73" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C76" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
         <v>25</v>
       </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
       <c r="C78" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" t="s">
         <v>29</v>
       </c>
-      <c r="B81" t="s">
-        <v>7</v>
-      </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1403,21 +1418,21 @@
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1425,76 +1440,76 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B86" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1502,43 +1517,43 @@
         <v>13</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B93" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C93" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1546,32 +1561,32 @@
         <v>14</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B97" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C97" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1579,21 +1594,21 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C99" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1601,21 +1616,21 @@
         <v>7</v>
       </c>
       <c r="B100" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1623,21 +1638,21 @@
         <v>4</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C102" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1645,43 +1660,43 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C104" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B105" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B106" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C106" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B107" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1689,21 +1704,21 @@
         <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B109" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C109" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1711,10 +1726,10 @@
         <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1722,43 +1737,43 @@
         <v>13</v>
       </c>
       <c r="B111" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C111" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C112" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B114" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C114" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1766,120 +1781,120 @@
         <v>14</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C115" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C116" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B117" t="s">
         <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C118" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B119" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C119" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C120" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B121" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C121" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B122" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B123" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C123" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B124" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C124" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B125" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C125" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1887,131 +1902,131 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C127" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C128" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C129" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B130" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C130" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B131" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C131" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B132" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C132" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C133" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B134" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C134" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C135" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C136" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B137" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C137" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -2019,10 +2034,10 @@
         <v>9</v>
       </c>
       <c r="B138" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C138" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -2030,10 +2045,10 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C139" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -2041,32 +2056,32 @@
         <v>13</v>
       </c>
       <c r="B140" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C140" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B141" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C141" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B142" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C142" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2074,54 +2089,54 @@
         <v>4</v>
       </c>
       <c r="B143" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C143" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B144" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C144" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B145" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B146" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C146" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B147" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C147" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2129,65 +2144,65 @@
         <v>6</v>
       </c>
       <c r="B148" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C148" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C149" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C150" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C151" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B152" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C152" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B153" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -2195,10 +2210,10 @@
         <v>14</v>
       </c>
       <c r="B154" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C154" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -2206,461 +2221,241 @@
         <v>10</v>
       </c>
       <c r="B155" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C155" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B156" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C156" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B157" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B158" t="s">
         <v>27</v>
       </c>
       <c r="C158" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C159" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B160" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C160" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B161" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C161" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B162" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C162" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B163" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C163" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B164" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C164" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B165" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C165" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B166" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C166" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C167" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B168" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C168" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B169" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C169" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B170" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C170" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B171" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C171" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
+        <v>27</v>
+      </c>
+      <c r="B172" t="s">
         <v>23</v>
       </c>
-      <c r="B172" t="s">
-        <v>21</v>
-      </c>
       <c r="C172" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B173" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C173" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B174" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B175" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C175" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B176" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C176" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="A177" t="s">
-        <v>25</v>
-      </c>
-      <c r="B177" t="s">
-        <v>4</v>
-      </c>
-      <c r="C177" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178" t="s">
-        <v>6</v>
-      </c>
-      <c r="B178" t="s">
-        <v>29</v>
-      </c>
-      <c r="C178" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179" t="s">
-        <v>23</v>
-      </c>
-      <c r="B179" t="s">
-        <v>26</v>
-      </c>
-      <c r="C179" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180" t="s">
-        <v>18</v>
-      </c>
-      <c r="B180" t="s">
-        <v>21</v>
-      </c>
-      <c r="C180" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181" t="s">
-        <v>3</v>
-      </c>
-      <c r="B181" t="s">
-        <v>24</v>
-      </c>
-      <c r="C181" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" t="s">
-        <v>27</v>
-      </c>
-      <c r="B182" t="s">
-        <v>7</v>
-      </c>
-      <c r="C182" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="A183" t="s">
-        <v>16</v>
-      </c>
-      <c r="B183" t="s">
-        <v>28</v>
-      </c>
-      <c r="C183" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" t="s">
-        <v>14</v>
-      </c>
-      <c r="B184" t="s">
-        <v>13</v>
-      </c>
-      <c r="C184" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" t="s">
-        <v>10</v>
-      </c>
-      <c r="B185" t="s">
-        <v>9</v>
-      </c>
-      <c r="C185" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" t="s">
-        <v>20</v>
-      </c>
-      <c r="B186" t="s">
-        <v>19</v>
-      </c>
-      <c r="C186" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" t="s">
-        <v>21</v>
-      </c>
-      <c r="B187" t="s">
-        <v>25</v>
-      </c>
-      <c r="C187" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188" t="s">
-        <v>9</v>
-      </c>
-      <c r="B188" t="s">
-        <v>23</v>
-      </c>
-      <c r="C188" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" t="s">
-        <v>7</v>
-      </c>
-      <c r="B189" t="s">
-        <v>16</v>
-      </c>
-      <c r="C189" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>13</v>
-      </c>
-      <c r="B190" t="s">
-        <v>20</v>
-      </c>
-      <c r="C190" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" t="s">
-        <v>26</v>
-      </c>
-      <c r="B191" t="s">
-        <v>10</v>
-      </c>
-      <c r="C191" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192" t="s">
-        <v>29</v>
-      </c>
-      <c r="B192" t="s">
-        <v>18</v>
-      </c>
-      <c r="C192" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" t="s">
-        <v>4</v>
-      </c>
-      <c r="B193" t="s">
-        <v>3</v>
-      </c>
-      <c r="C193" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194" t="s">
-        <v>28</v>
-      </c>
-      <c r="B194" t="s">
-        <v>6</v>
-      </c>
-      <c r="C194" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195" t="s">
-        <v>19</v>
-      </c>
-      <c r="B195" t="s">
-        <v>14</v>
-      </c>
-      <c r="C195" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>24</v>
-      </c>
-      <c r="B196" t="s">
-        <v>27</v>
-      </c>
-      <c r="C196" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>